<commit_message>
up new ERP Note
</commit_message>
<xml_diff>
--- a/MyExcel.xlsx
+++ b/MyExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoo_Note\Up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7233532E-96DD-4564-A8D7-2787D35897CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEAEAB7-986B-4543-AF09-B34B57A7DFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{7CF9CE48-03F9-4D46-B430-5B04D272F059}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="121">
   <si>
     <t>Table</t>
   </si>
@@ -261,7 +261,133 @@
     <t>MVFILEM_BATCH</t>
   </si>
   <si>
-    <t>Documentation -&gt; Batch Update Vehicle File Movement (7)</t>
+    <t>Documentation -&gt; Batch Update Vehicle File Movement (10)</t>
+  </si>
+  <si>
+    <t>Spare Parts</t>
+  </si>
+  <si>
+    <t>MITEM_SP</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Setup -&gt; Item Master (1)</t>
+  </si>
+  <si>
+    <t>MSTORE_SP</t>
+  </si>
+  <si>
+    <t>MLOC_SP</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Setup -&gt; Store Setup (2)</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Setup -&gt; Location Setup (3)</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Setup -&gt; Item Group (3)</t>
+  </si>
+  <si>
+    <t>MITEMGROUP</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InfoHSA / </t>
+  </si>
+  <si>
+    <t>MSUBGRP</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Setup -&gt; Sub Group (5)</t>
+  </si>
+  <si>
+    <t>MBRAND</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Setup -&gt; Brand (6)</t>
+  </si>
+  <si>
+    <t>MGROUP</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Setup -&gt; Group (6)</t>
+  </si>
+  <si>
+    <t>SGRN_SP</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Good Receive Note (2)</t>
+  </si>
+  <si>
+    <t>LSI</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Delivery Order (3)</t>
+  </si>
+  <si>
+    <t>SBC_SP</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Store Bin Card (4)</t>
+  </si>
+  <si>
+    <t>ON / OFF</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>SIR_SP</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Stock Adjustment (5)</t>
+  </si>
+  <si>
+    <t>BST_SP</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Branch Stock Transfer (6)</t>
+  </si>
+  <si>
+    <t>INTERNAL_USE</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Internal Use v2 (7)</t>
+  </si>
+  <si>
+    <t>INTERNAL_USE_SABAH</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Internal Use v1 (8)</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Internal Use (9)</t>
+  </si>
+  <si>
+    <t>SRQ_SP</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Parts Request (10)</t>
+  </si>
+  <si>
+    <t>RSTOCK_BAL</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Report -&gt; Stock Balance Report (1)</t>
+  </si>
+  <si>
+    <t>RSTOCK_COST_DATE</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Report -&gt; Stock Balance By Date Report (2)</t>
+  </si>
+  <si>
+    <t>RSALES_SUM</t>
+  </si>
+  <si>
+    <t>Spare Parts -&gt; Report -&gt; Sales Summary Report (3)</t>
   </si>
 </sst>
 </file>
@@ -333,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,6 +471,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -370,6 +502,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,8 +564,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{85B26E9C-34CE-4A87-A053-77F71710B357}" name="Table4" displayName="Table4" ref="A2:E17" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A2:E17" xr:uid="{85B26E9C-34CE-4A87-A053-77F71710B357}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{85B26E9C-34CE-4A87-A053-77F71710B357}" name="Table4" displayName="Table4" ref="A2:E25" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A2:E25" xr:uid="{85B26E9C-34CE-4A87-A053-77F71710B357}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C74E7030-1C55-410C-9395-CFBCE335F1E4}" name="Table" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{7A01E317-2C37-44D7-A1FD-0190B7DD3582}" name="Link（ERP9）" dataDxfId="3"/>
@@ -425,12 +578,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E428264C-037D-4310-83D8-572E434224C5}" name="Table6" displayName="Table6" ref="A20:C44" totalsRowShown="0">
-  <autoFilter ref="A20:C44" xr:uid="{E428264C-037D-4310-83D8-572E434224C5}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E428264C-037D-4310-83D8-572E434224C5}" name="Table6" displayName="Table6" ref="A28:D66" totalsRowShown="0">
+  <autoFilter ref="A28:D66" xr:uid="{E428264C-037D-4310-83D8-572E434224C5}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5C414036-DD3F-4615-BE4E-BD9541BD0B0B}" name="Tables"/>
     <tableColumn id="2" xr3:uid="{7B03EA7E-97B9-431B-98B7-23D2AD1C72DE}" name="Link (ERP9)"/>
     <tableColumn id="3" xr3:uid="{7488F295-44FA-4375-81E1-0CAFD79EB382}" name="Des"/>
+    <tableColumn id="4" xr3:uid="{30862E24-D64D-4278-99F1-192393D77E1A}" name="ON / OFF"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -733,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD9FD1E-5655-431E-B85D-770A1A30F042}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,13 +903,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -777,16 +931,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -803,7 +957,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -816,19 +970,19 @@
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -845,7 +999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -863,15 +1017,15 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -889,15 +1043,15 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -914,7 +1068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
@@ -932,15 +1086,15 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -957,7 +1111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>63</v>
       </c>
@@ -974,141 +1128,178 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B27" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C27" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B28" t="s">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C28" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="8" t="s">
+      <c r="D28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A29" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A27" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" t="s">
-        <v>51</v>
+        <v>30</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>23</v>
@@ -1116,28 +1307,32 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" t="s">
-        <v>70</v>
+        <v>33</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A32" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
+        <v>37</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>23</v>
@@ -1145,108 +1340,377 @@
     </row>
     <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" t="s">
-        <v>56</v>
+        <v>43</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>23</v>
-      </c>
+    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A35" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" t="s">
-        <v>60</v>
+        <v>45</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A37" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" t="s">
-        <v>66</v>
+        <v>49</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A39" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A41" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="4" t="s">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A40" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="11"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A45" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="21"/>
+      <c r="C45" s="15"/>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A47" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="21"/>
+      <c r="C47" s="15"/>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A49" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="21"/>
+      <c r="C49" s="15"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B51" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A44" s="10" t="s">
+      <c r="C51" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A52" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="21"/>
+      <c r="C52" s="15"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C64" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A66" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>